<commit_message>
scada files fetch script done
</commit_message>
<xml_diff>
--- a/python_report/state_files/IRE.xlsx
+++ b/python_report/state_files/IRE.xlsx
@@ -1199,6 +1199,114 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="6" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
@@ -1237,114 +1345,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1634,8 +1634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="73" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="73" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1668,17 +1668,17 @@
       <c r="K1" s="41"/>
     </row>
     <row r="2" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="145" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="145"/>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="145"/>
-      <c r="F2" s="145"/>
-      <c r="G2" s="145"/>
-      <c r="H2" s="145"/>
-      <c r="I2" s="145"/>
+      <c r="A2" s="137" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="137"/>
+      <c r="C2" s="137"/>
+      <c r="D2" s="137"/>
+      <c r="E2" s="137"/>
+      <c r="F2" s="137"/>
+      <c r="G2" s="137"/>
+      <c r="H2" s="137"/>
+      <c r="I2" s="137"/>
       <c r="J2" s="40"/>
       <c r="K2" s="41"/>
     </row>
@@ -1689,13 +1689,13 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="146" t="s">
+      <c r="G3" s="138" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="147"/>
-      <c r="I3" s="147"/>
-      <c r="J3" s="147"/>
-      <c r="K3" s="148"/>
+      <c r="H3" s="139"/>
+      <c r="I3" s="139"/>
+      <c r="J3" s="139"/>
+      <c r="K3" s="140"/>
     </row>
     <row r="4" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
@@ -1710,11 +1710,11 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="149"/>
-      <c r="H4" s="150"/>
-      <c r="I4" s="150"/>
-      <c r="J4" s="150"/>
-      <c r="K4" s="151"/>
+      <c r="G4" s="141"/>
+      <c r="H4" s="142"/>
+      <c r="I4" s="142"/>
+      <c r="J4" s="142"/>
+      <c r="K4" s="143"/>
     </row>
     <row r="5" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="8"/>
@@ -1723,11 +1723,11 @@
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
-      <c r="G5" s="152"/>
-      <c r="H5" s="153"/>
-      <c r="I5" s="153"/>
-      <c r="J5" s="153"/>
-      <c r="K5" s="154"/>
+      <c r="G5" s="144"/>
+      <c r="H5" s="145"/>
+      <c r="I5" s="145"/>
+      <c r="J5" s="145"/>
+      <c r="K5" s="146"/>
     </row>
     <row r="6" spans="1:11" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="8"/>
@@ -1743,51 +1743,51 @@
       <c r="K6" s="43"/>
     </row>
     <row r="7" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="155" t="s">
+      <c r="A7" s="147" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="155"/>
-      <c r="C7" s="156"/>
-      <c r="D7" s="156"/>
-      <c r="E7" s="156"/>
-      <c r="F7" s="156"/>
-      <c r="G7" s="157"/>
-      <c r="H7" s="158" t="s">
+      <c r="B7" s="147"/>
+      <c r="C7" s="148"/>
+      <c r="D7" s="148"/>
+      <c r="E7" s="148"/>
+      <c r="F7" s="148"/>
+      <c r="G7" s="149"/>
+      <c r="H7" s="150" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="159"/>
-      <c r="J7" s="159"/>
-      <c r="K7" s="160"/>
+      <c r="I7" s="151"/>
+      <c r="J7" s="151"/>
+      <c r="K7" s="152"/>
     </row>
     <row r="8" spans="1:11" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="155" t="s">
+      <c r="A8" s="147" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="164"/>
-      <c r="C8" s="165" t="s">
+      <c r="B8" s="156"/>
+      <c r="C8" s="157" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="165"/>
-      <c r="E8" s="165"/>
-      <c r="F8" s="165"/>
-      <c r="G8" s="157"/>
-      <c r="H8" s="161"/>
-      <c r="I8" s="162"/>
-      <c r="J8" s="162"/>
-      <c r="K8" s="163"/>
+      <c r="D8" s="157"/>
+      <c r="E8" s="157"/>
+      <c r="F8" s="157"/>
+      <c r="G8" s="149"/>
+      <c r="H8" s="153"/>
+      <c r="I8" s="154"/>
+      <c r="J8" s="154"/>
+      <c r="K8" s="155"/>
     </row>
     <row r="9" spans="1:11" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="155"/>
-      <c r="B9" s="164"/>
-      <c r="C9" s="165" t="s">
+      <c r="A9" s="147"/>
+      <c r="B9" s="156"/>
+      <c r="C9" s="157" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="165"/>
-      <c r="E9" s="165" t="s">
+      <c r="D9" s="157"/>
+      <c r="E9" s="157" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="165"/>
-      <c r="G9" s="157"/>
+      <c r="F9" s="157"/>
+      <c r="G9" s="149"/>
       <c r="H9" s="127" t="s">
         <v>10</v>
       </c>
@@ -1802,8 +1802,8 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="155"/>
-      <c r="B10" s="164"/>
+      <c r="A10" s="147"/>
+      <c r="B10" s="156"/>
       <c r="C10" s="11" t="s">
         <v>12</v>
       </c>
@@ -1816,22 +1816,22 @@
       <c r="F10" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="157"/>
+      <c r="G10" s="149"/>
       <c r="H10" s="129" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="180">
+      <c r="I10" s="136">
         <v>792</v>
       </c>
-      <c r="J10" s="180">
+      <c r="J10" s="136">
         <v>804</v>
       </c>
-      <c r="K10" s="180">
+      <c r="K10" s="136">
         <v>803</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="166" t="s">
+      <c r="A11" s="158" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="13" t="s">
@@ -1847,7 +1847,7 @@
       <c r="F11" s="105">
         <v>-5.25</v>
       </c>
-      <c r="G11" s="157"/>
+      <c r="G11" s="149"/>
       <c r="H11" s="129" t="s">
         <v>17</v>
       </c>
@@ -1862,7 +1862,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="166"/>
+      <c r="A12" s="158"/>
       <c r="B12" s="13" t="s">
         <v>18</v>
       </c>
@@ -1872,7 +1872,7 @@
       </c>
       <c r="E12" s="106"/>
       <c r="F12" s="102"/>
-      <c r="G12" s="157"/>
+      <c r="G12" s="149"/>
       <c r="H12" s="129" t="s">
         <v>19</v>
       </c>
@@ -1887,7 +1887,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="167" t="s">
+      <c r="A13" s="159" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="14" t="s">
@@ -1901,7 +1901,7 @@
       <c r="F13" s="121">
         <v>0</v>
       </c>
-      <c r="G13" s="157"/>
+      <c r="G13" s="149"/>
       <c r="H13" s="130" t="s">
         <v>17</v>
       </c>
@@ -1916,7 +1916,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="166"/>
+      <c r="A14" s="158"/>
       <c r="B14" s="13" t="s">
         <v>18</v>
       </c>
@@ -1924,14 +1924,14 @@
       <c r="D14" s="99"/>
       <c r="E14" s="99"/>
       <c r="F14" s="106"/>
-      <c r="G14" s="157"/>
+      <c r="G14" s="149"/>
       <c r="H14" s="45"/>
       <c r="I14" s="46"/>
       <c r="J14" s="47"/>
       <c r="K14" s="47"/>
     </row>
     <row r="15" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A15" s="168" t="s">
+      <c r="A15" s="160" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="13" t="s">
@@ -1949,14 +1949,14 @@
       <c r="F15" s="107">
         <v>0</v>
       </c>
-      <c r="G15" s="157"/>
+      <c r="G15" s="149"/>
       <c r="H15" s="45"/>
       <c r="I15" s="48"/>
       <c r="J15" s="45"/>
       <c r="K15" s="49"/>
     </row>
     <row r="16" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A16" s="168"/>
+      <c r="A16" s="160"/>
       <c r="B16" s="15" t="s">
         <v>18</v>
       </c>
@@ -1968,14 +1968,14 @@
       </c>
       <c r="E16" s="101"/>
       <c r="F16" s="107"/>
-      <c r="G16" s="157"/>
+      <c r="G16" s="149"/>
       <c r="H16" s="45"/>
       <c r="I16" s="48"/>
       <c r="J16" s="45"/>
       <c r="K16" s="49"/>
     </row>
     <row r="17" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A17" s="168"/>
+      <c r="A17" s="160"/>
       <c r="B17" s="13" t="s">
         <v>23</v>
       </c>
@@ -1991,14 +1991,14 @@
       <c r="F17" s="107">
         <v>0</v>
       </c>
-      <c r="G17" s="157"/>
+      <c r="G17" s="149"/>
       <c r="H17" s="45"/>
       <c r="I17" s="48"/>
       <c r="J17" s="45"/>
       <c r="K17" s="49"/>
     </row>
     <row r="18" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A18" s="168"/>
+      <c r="A18" s="160"/>
       <c r="B18" s="15" t="s">
         <v>18</v>
       </c>
@@ -2010,14 +2010,14 @@
       </c>
       <c r="E18" s="101"/>
       <c r="F18" s="103"/>
-      <c r="G18" s="157"/>
+      <c r="G18" s="149"/>
       <c r="H18" s="45"/>
       <c r="I18" s="48"/>
       <c r="J18" s="45"/>
       <c r="K18" s="49"/>
     </row>
     <row r="19" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="168"/>
+      <c r="A19" s="160"/>
       <c r="B19" s="37" t="s">
         <v>24</v>
       </c>
@@ -2031,14 +2031,14 @@
       <c r="F19" s="103">
         <v>0</v>
       </c>
-      <c r="G19" s="157"/>
+      <c r="G19" s="149"/>
       <c r="H19" s="50"/>
       <c r="I19" s="50"/>
       <c r="J19" s="50"/>
       <c r="K19" s="50"/>
     </row>
     <row r="20" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A20" s="168"/>
+      <c r="A20" s="160"/>
       <c r="B20" s="38" t="s">
         <v>18</v>
       </c>
@@ -2048,14 +2048,14 @@
       <c r="D20" s="103"/>
       <c r="E20" s="107"/>
       <c r="F20" s="103"/>
-      <c r="G20" s="157"/>
+      <c r="G20" s="149"/>
       <c r="H20" s="45"/>
       <c r="I20" s="48"/>
       <c r="J20" s="45"/>
       <c r="K20" s="49"/>
     </row>
     <row r="21" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="168"/>
+      <c r="A21" s="160"/>
       <c r="B21" s="37" t="s">
         <v>25</v>
       </c>
@@ -2069,14 +2069,14 @@
       <c r="F21" s="103">
         <v>0</v>
       </c>
-      <c r="G21" s="157"/>
+      <c r="G21" s="149"/>
       <c r="H21" s="45"/>
       <c r="I21" s="48"/>
       <c r="J21" s="45"/>
       <c r="K21" s="49"/>
     </row>
     <row r="22" spans="1:11" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="168"/>
+      <c r="A22" s="160"/>
       <c r="B22" s="16" t="s">
         <v>18</v>
       </c>
@@ -2086,14 +2086,14 @@
       <c r="D22" s="103"/>
       <c r="E22" s="103"/>
       <c r="F22" s="103"/>
-      <c r="G22" s="157"/>
+      <c r="G22" s="149"/>
       <c r="H22" s="45"/>
       <c r="I22" s="48"/>
       <c r="J22" s="45"/>
       <c r="K22" s="49"/>
     </row>
     <row r="23" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="168" t="s">
+      <c r="A23" s="160" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="17" t="s">
@@ -2109,16 +2109,16 @@
       <c r="F23" s="108">
         <v>-4.8329000000000004</v>
       </c>
-      <c r="G23" s="157"/>
-      <c r="H23" s="169" t="s">
+      <c r="G23" s="149"/>
+      <c r="H23" s="161" t="s">
         <v>28</v>
       </c>
-      <c r="I23" s="170"/>
-      <c r="J23" s="171"/>
+      <c r="I23" s="162"/>
+      <c r="J23" s="163"/>
       <c r="K23" s="51"/>
     </row>
     <row r="24" spans="1:11" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="168"/>
+      <c r="A24" s="160"/>
       <c r="B24" s="17" t="s">
         <v>18</v>
       </c>
@@ -2128,14 +2128,14 @@
       </c>
       <c r="E24" s="101"/>
       <c r="F24" s="109"/>
-      <c r="G24" s="157"/>
-      <c r="H24" s="172"/>
-      <c r="I24" s="173"/>
-      <c r="J24" s="174"/>
+      <c r="G24" s="149"/>
+      <c r="H24" s="164"/>
+      <c r="I24" s="165"/>
+      <c r="J24" s="166"/>
       <c r="K24" s="51"/>
     </row>
-    <row r="25" spans="1:11" ht="68.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="168"/>
+    <row r="25" spans="1:11" ht="47.25" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="160"/>
       <c r="B25" s="17" t="s">
         <v>29</v>
       </c>
@@ -2149,7 +2149,7 @@
       <c r="F25" s="109">
         <v>-4.9703999999999997</v>
       </c>
-      <c r="G25" s="157"/>
+      <c r="G25" s="149"/>
       <c r="H25" s="52" t="s">
         <v>10</v>
       </c>
@@ -2162,7 +2162,7 @@
       <c r="K25" s="54"/>
     </row>
     <row r="26" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="168"/>
+      <c r="A26" s="160"/>
       <c r="B26" s="18" t="s">
         <v>18</v>
       </c>
@@ -2172,7 +2172,7 @@
       </c>
       <c r="E26" s="106"/>
       <c r="F26" s="110"/>
-      <c r="G26" s="157"/>
+      <c r="G26" s="149"/>
       <c r="H26" s="55" t="s">
         <v>14</v>
       </c>
@@ -2185,7 +2185,7 @@
       <c r="K26" s="58"/>
     </row>
     <row r="27" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="168"/>
+      <c r="A27" s="160"/>
       <c r="B27" s="34" t="s">
         <v>31</v>
       </c>
@@ -2199,7 +2199,7 @@
       <c r="F27" s="110">
         <v>-3.673</v>
       </c>
-      <c r="G27" s="157"/>
+      <c r="G27" s="149"/>
       <c r="H27" s="59" t="s">
         <v>17</v>
       </c>
@@ -2212,7 +2212,7 @@
       <c r="K27" s="62"/>
     </row>
     <row r="28" spans="1:11" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="168"/>
+      <c r="A28" s="160"/>
       <c r="B28" s="35" t="s">
         <v>18</v>
       </c>
@@ -2222,7 +2222,7 @@
       </c>
       <c r="E28" s="106"/>
       <c r="F28" s="110"/>
-      <c r="G28" s="157"/>
+      <c r="G28" s="149"/>
       <c r="H28" s="59" t="s">
         <v>19</v>
       </c>
@@ -2235,7 +2235,7 @@
       <c r="K28" s="64"/>
     </row>
     <row r="29" spans="1:11" ht="47.25" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="168"/>
+      <c r="A29" s="160"/>
       <c r="B29" s="36" t="s">
         <v>32</v>
       </c>
@@ -2249,7 +2249,7 @@
       <c r="F29" s="110">
         <v>-3.7726999999999999</v>
       </c>
-      <c r="G29" s="157"/>
+      <c r="G29" s="149"/>
       <c r="H29" s="65" t="s">
         <v>17</v>
       </c>
@@ -2262,7 +2262,7 @@
       <c r="K29" s="62"/>
     </row>
     <row r="30" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A30" s="168"/>
+      <c r="A30" s="160"/>
       <c r="B30" s="18" t="s">
         <v>18</v>
       </c>
@@ -2272,14 +2272,14 @@
       </c>
       <c r="E30" s="101"/>
       <c r="F30" s="109"/>
-      <c r="G30" s="157"/>
+      <c r="G30" s="149"/>
       <c r="H30" s="58"/>
       <c r="I30" s="66"/>
       <c r="J30" s="67"/>
       <c r="K30" s="67"/>
     </row>
     <row r="31" spans="1:11" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="168"/>
+      <c r="A31" s="160"/>
       <c r="B31" s="24" t="s">
         <v>61</v>
       </c>
@@ -2289,14 +2289,14 @@
       </c>
       <c r="E31" s="100"/>
       <c r="F31" s="103"/>
-      <c r="G31" s="157"/>
+      <c r="G31" s="149"/>
       <c r="H31" s="58"/>
       <c r="I31" s="67"/>
       <c r="J31" s="66"/>
       <c r="K31" s="67"/>
     </row>
     <row r="32" spans="1:11" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="168"/>
+      <c r="A32" s="160"/>
       <c r="B32" s="24" t="s">
         <v>18</v>
       </c>
@@ -2304,14 +2304,14 @@
       <c r="D32" s="101"/>
       <c r="E32" s="101"/>
       <c r="F32" s="101"/>
-      <c r="G32" s="157"/>
+      <c r="G32" s="149"/>
       <c r="H32" s="58"/>
       <c r="I32" s="68"/>
       <c r="J32" s="69"/>
       <c r="K32" s="67"/>
     </row>
     <row r="33" spans="1:11" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="168"/>
+      <c r="A33" s="160"/>
       <c r="B33" s="24" t="s">
         <v>62</v>
       </c>
@@ -2321,14 +2321,14 @@
       </c>
       <c r="E33" s="100"/>
       <c r="F33" s="103"/>
-      <c r="G33" s="157"/>
+      <c r="G33" s="149"/>
       <c r="H33" s="58"/>
       <c r="I33" s="68"/>
       <c r="J33" s="69"/>
       <c r="K33" s="67"/>
     </row>
     <row r="34" spans="1:11" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A34" s="168"/>
+      <c r="A34" s="160"/>
       <c r="B34" s="24" t="s">
         <v>18</v>
       </c>
@@ -2336,14 +2336,14 @@
       <c r="D34" s="112"/>
       <c r="E34" s="113"/>
       <c r="F34" s="114"/>
-      <c r="G34" s="157"/>
+      <c r="G34" s="149"/>
       <c r="H34" s="58"/>
       <c r="I34" s="68"/>
       <c r="J34" s="69"/>
       <c r="K34" s="67"/>
     </row>
     <row r="35" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A35" s="168"/>
+      <c r="A35" s="160"/>
       <c r="B35" s="19" t="s">
         <v>33</v>
       </c>
@@ -2357,14 +2357,14 @@
       <c r="F35" s="104">
         <v>-5.0140000000000002</v>
       </c>
-      <c r="G35" s="157"/>
+      <c r="G35" s="149"/>
       <c r="H35" s="58"/>
       <c r="I35" s="68"/>
       <c r="J35" s="68"/>
       <c r="K35" s="67"/>
     </row>
     <row r="36" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A36" s="168"/>
+      <c r="A36" s="160"/>
       <c r="B36" s="19" t="s">
         <v>18</v>
       </c>
@@ -2374,14 +2374,14 @@
       </c>
       <c r="E36" s="104"/>
       <c r="F36" s="104"/>
-      <c r="G36" s="157"/>
+      <c r="G36" s="149"/>
       <c r="H36" s="67"/>
       <c r="I36" s="43"/>
       <c r="J36" s="43"/>
       <c r="K36" s="43"/>
     </row>
     <row r="37" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="168"/>
+      <c r="A37" s="160"/>
       <c r="B37" s="17" t="s">
         <v>34</v>
       </c>
@@ -2395,14 +2395,14 @@
       <c r="F37" s="104">
         <v>-4.1929999999999996</v>
       </c>
-      <c r="G37" s="157"/>
+      <c r="G37" s="149"/>
       <c r="H37" s="67"/>
       <c r="I37" s="43"/>
       <c r="J37" s="43"/>
       <c r="K37" s="43"/>
     </row>
     <row r="38" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A38" s="168"/>
+      <c r="A38" s="160"/>
       <c r="B38" s="19" t="s">
         <v>18</v>
       </c>
@@ -2412,14 +2412,14 @@
       </c>
       <c r="E38" s="101"/>
       <c r="F38" s="101"/>
-      <c r="G38" s="157"/>
+      <c r="G38" s="149"/>
       <c r="H38" s="67"/>
       <c r="I38" s="43"/>
       <c r="J38" s="43"/>
       <c r="K38" s="43"/>
     </row>
     <row r="39" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="168"/>
+      <c r="A39" s="160"/>
       <c r="B39" s="17" t="s">
         <v>35</v>
       </c>
@@ -2433,16 +2433,16 @@
       <c r="F39" s="104">
         <v>-3.7349999999999999</v>
       </c>
-      <c r="G39" s="157"/>
+      <c r="G39" s="149"/>
       <c r="H39" s="58"/>
-      <c r="I39" s="175" t="s">
+      <c r="I39" s="167" t="s">
         <v>36</v>
       </c>
-      <c r="J39" s="175"/>
+      <c r="J39" s="167"/>
       <c r="K39" s="43"/>
     </row>
     <row r="40" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A40" s="168"/>
+      <c r="A40" s="160"/>
       <c r="B40" s="19" t="s">
         <v>18</v>
       </c>
@@ -2452,7 +2452,7 @@
       </c>
       <c r="E40" s="101"/>
       <c r="F40" s="101"/>
-      <c r="G40" s="157"/>
+      <c r="G40" s="149"/>
       <c r="H40" s="58"/>
       <c r="I40" s="70" t="s">
         <v>37</v>
@@ -2461,7 +2461,7 @@
       <c r="K40" s="43"/>
     </row>
     <row r="41" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="168"/>
+      <c r="A41" s="160"/>
       <c r="B41" s="17" t="s">
         <v>38</v>
       </c>
@@ -2475,14 +2475,14 @@
       <c r="F41" s="116">
         <v>-8.827</v>
       </c>
-      <c r="G41" s="157"/>
+      <c r="G41" s="149"/>
       <c r="H41" s="58"/>
       <c r="I41" s="43"/>
       <c r="J41" s="43"/>
       <c r="K41" s="43"/>
     </row>
     <row r="42" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A42" s="168"/>
+      <c r="A42" s="160"/>
       <c r="B42" s="19" t="s">
         <v>18</v>
       </c>
@@ -2492,14 +2492,14 @@
       </c>
       <c r="E42" s="101"/>
       <c r="F42" s="101"/>
-      <c r="G42" s="157"/>
+      <c r="G42" s="149"/>
       <c r="H42" s="58"/>
       <c r="I42" s="43"/>
       <c r="J42" s="43"/>
       <c r="K42" s="43"/>
     </row>
     <row r="43" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="168"/>
+      <c r="A43" s="160"/>
       <c r="B43" s="17" t="s">
         <v>39</v>
       </c>
@@ -2513,14 +2513,14 @@
       <c r="F43" s="100">
         <v>-8.7270000000000003</v>
       </c>
-      <c r="G43" s="157"/>
+      <c r="G43" s="149"/>
       <c r="H43" s="58"/>
       <c r="I43" s="43"/>
       <c r="J43" s="43"/>
       <c r="K43" s="43"/>
     </row>
     <row r="44" spans="1:11" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="168"/>
+      <c r="A44" s="160"/>
       <c r="B44" s="19" t="s">
         <v>18</v>
       </c>
@@ -2530,14 +2530,14 @@
       </c>
       <c r="E44" s="101"/>
       <c r="F44" s="103"/>
-      <c r="G44" s="157"/>
+      <c r="G44" s="149"/>
       <c r="H44" s="71"/>
       <c r="I44" s="43"/>
       <c r="J44" s="53"/>
       <c r="K44" s="72"/>
     </row>
     <row r="45" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A45" s="132" t="s">
+      <c r="A45" s="168" t="s">
         <v>40</v>
       </c>
       <c r="B45" s="19" t="s">
@@ -2547,20 +2547,20 @@
       <c r="D45" s="83">
         <v>-1667</v>
       </c>
-      <c r="E45" s="176">
+      <c r="E45" s="132">
         <v>0</v>
       </c>
       <c r="F45" s="84">
         <v>-26.158000000000001</v>
       </c>
-      <c r="G45" s="133"/>
-      <c r="H45" s="133"/>
-      <c r="I45" s="133"/>
-      <c r="J45" s="133"/>
-      <c r="K45" s="133"/>
+      <c r="G45" s="169"/>
+      <c r="H45" s="169"/>
+      <c r="I45" s="169"/>
+      <c r="J45" s="169"/>
+      <c r="K45" s="169"/>
     </row>
     <row r="46" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A46" s="132"/>
+      <c r="A46" s="168"/>
       <c r="B46" s="19" t="s">
         <v>18</v>
       </c>
@@ -2577,7 +2577,7 @@
       <c r="K46" s="71"/>
     </row>
     <row r="47" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A47" s="132"/>
+      <c r="A47" s="168"/>
       <c r="B47" s="19" t="s">
         <v>42</v>
       </c>
@@ -2598,7 +2598,7 @@
       <c r="K47" s="71"/>
     </row>
     <row r="48" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A48" s="132"/>
+      <c r="A48" s="168"/>
       <c r="B48" s="17" t="s">
         <v>18</v>
       </c>
@@ -2615,7 +2615,7 @@
       <c r="K48" s="71"/>
     </row>
     <row r="49" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A49" s="132"/>
+      <c r="A49" s="168"/>
       <c r="B49" s="19" t="s">
         <v>43</v>
       </c>
@@ -2636,7 +2636,7 @@
       <c r="K49" s="71"/>
     </row>
     <row r="50" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A50" s="132"/>
+      <c r="A50" s="168"/>
       <c r="B50" s="17" t="s">
         <v>18</v>
       </c>
@@ -2653,7 +2653,7 @@
       <c r="K50" s="71"/>
     </row>
     <row r="51" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A51" s="132"/>
+      <c r="A51" s="168"/>
       <c r="B51" s="20" t="s">
         <v>44</v>
       </c>
@@ -2674,7 +2674,7 @@
       <c r="K51" s="71"/>
     </row>
     <row r="52" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A52" s="132"/>
+      <c r="A52" s="168"/>
       <c r="B52" s="21" t="s">
         <v>18</v>
       </c>
@@ -2691,7 +2691,7 @@
       <c r="K52" s="71"/>
     </row>
     <row r="53" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A53" s="132"/>
+      <c r="A53" s="168"/>
       <c r="B53" s="20" t="s">
         <v>45</v>
       </c>
@@ -2712,7 +2712,7 @@
       <c r="K53" s="71"/>
     </row>
     <row r="54" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A54" s="132"/>
+      <c r="A54" s="168"/>
       <c r="B54" s="21" t="s">
         <v>18</v>
       </c>
@@ -2729,7 +2729,7 @@
       <c r="K54" s="71"/>
     </row>
     <row r="55" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A55" s="132"/>
+      <c r="A55" s="168"/>
       <c r="B55" s="22" t="s">
         <v>46</v>
       </c>
@@ -2738,10 +2738,10 @@
         <f>-714*2</f>
         <v>-1428</v>
       </c>
-      <c r="E55" s="177">
-        <v>0</v>
-      </c>
-      <c r="F55" s="178">
+      <c r="E55" s="133">
+        <v>0</v>
+      </c>
+      <c r="F55" s="134">
         <v>-21.972000000000001</v>
       </c>
       <c r="G55" s="67"/>
@@ -2751,7 +2751,7 @@
       <c r="K55" s="41"/>
     </row>
     <row r="56" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A56" s="132"/>
+      <c r="A56" s="168"/>
       <c r="B56" s="22" t="s">
         <v>18</v>
       </c>
@@ -2768,7 +2768,7 @@
       <c r="K56" s="41"/>
     </row>
     <row r="57" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A57" s="137"/>
+      <c r="A57" s="173"/>
       <c r="B57" s="22" t="s">
         <v>47</v>
       </c>
@@ -2791,7 +2791,7 @@
       <c r="K57" s="41"/>
     </row>
     <row r="58" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A58" s="137"/>
+      <c r="A58" s="173"/>
       <c r="B58" s="22" t="s">
         <v>18</v>
       </c>
@@ -2810,7 +2810,7 @@
       <c r="K58" s="41"/>
     </row>
     <row r="59" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A59" s="137"/>
+      <c r="A59" s="173"/>
       <c r="B59" s="22" t="s">
         <v>48</v>
       </c>
@@ -2833,7 +2833,7 @@
       <c r="K59" s="41"/>
     </row>
     <row r="60" spans="1:12" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A60" s="138"/>
+      <c r="A60" s="174"/>
       <c r="B60" s="23" t="s">
         <v>18</v>
       </c>
@@ -2852,7 +2852,7 @@
       <c r="K60" s="41"/>
     </row>
     <row r="61" spans="1:12" s="27" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A61" s="139" t="s">
+      <c r="A61" s="175" t="s">
         <v>49</v>
       </c>
       <c r="B61" s="26" t="s">
@@ -2876,7 +2876,7 @@
       <c r="L61" s="76"/>
     </row>
     <row r="62" spans="1:12" s="27" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A62" s="140"/>
+      <c r="A62" s="176"/>
       <c r="B62" s="28" t="s">
         <v>18</v>
       </c>
@@ -2894,7 +2894,7 @@
       <c r="L62" s="76"/>
     </row>
     <row r="63" spans="1:12" s="27" customFormat="1" ht="33" x14ac:dyDescent="0.3">
-      <c r="A63" s="140"/>
+      <c r="A63" s="176"/>
       <c r="B63" s="26" t="s">
         <v>51</v>
       </c>
@@ -2914,7 +2914,7 @@
       <c r="L63" s="76"/>
     </row>
     <row r="64" spans="1:12" s="27" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A64" s="141"/>
+      <c r="A64" s="177"/>
       <c r="B64" s="28" t="s">
         <v>18</v>
       </c>
@@ -2930,7 +2930,7 @@
       <c r="L64" s="76"/>
     </row>
     <row r="65" spans="1:12" s="27" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A65" s="142" t="s">
+      <c r="A65" s="178" t="s">
         <v>52</v>
       </c>
       <c r="B65" s="29" t="s">
@@ -2940,7 +2940,7 @@
       <c r="D65" s="104">
         <v>-970</v>
       </c>
-      <c r="E65" s="177">
+      <c r="E65" s="133">
         <v>0</v>
       </c>
       <c r="F65" s="117">
@@ -2954,7 +2954,7 @@
       <c r="L65" s="76"/>
     </row>
     <row r="66" spans="1:12" s="27" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A66" s="143"/>
+      <c r="A66" s="179"/>
       <c r="B66" s="30" t="s">
         <v>54</v>
       </c>
@@ -2972,7 +2972,7 @@
       <c r="L66" s="76"/>
     </row>
     <row r="67" spans="1:12" s="27" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A67" s="143"/>
+      <c r="A67" s="179"/>
       <c r="B67" s="29" t="s">
         <v>55</v>
       </c>
@@ -2994,7 +2994,7 @@
       <c r="L67" s="76"/>
     </row>
     <row r="68" spans="1:12" s="27" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A68" s="144"/>
+      <c r="A68" s="180"/>
       <c r="B68" s="30" t="s">
         <v>54</v>
       </c>
@@ -3012,7 +3012,7 @@
       <c r="L68" s="76"/>
     </row>
     <row r="69" spans="1:12" s="27" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A69" s="142" t="s">
+      <c r="A69" s="178" t="s">
         <v>56</v>
       </c>
       <c r="B69" s="29" t="s">
@@ -3022,7 +3022,7 @@
       <c r="D69" s="91">
         <v>-475</v>
       </c>
-      <c r="E69" s="179">
+      <c r="E69" s="135">
         <v>0</v>
       </c>
       <c r="F69" s="97">
@@ -3036,7 +3036,7 @@
       <c r="L69" s="76"/>
     </row>
     <row r="70" spans="1:12" s="27" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A70" s="143"/>
+      <c r="A70" s="179"/>
       <c r="B70" s="30" t="s">
         <v>54</v>
       </c>
@@ -3054,7 +3054,7 @@
       <c r="L70" s="76"/>
     </row>
     <row r="71" spans="1:12" s="27" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A71" s="143"/>
+      <c r="A71" s="179"/>
       <c r="B71" s="29" t="s">
         <v>58</v>
       </c>
@@ -3076,7 +3076,7 @@
       <c r="L71" s="76"/>
     </row>
     <row r="72" spans="1:12" s="27" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A72" s="144"/>
+      <c r="A72" s="180"/>
       <c r="B72" s="30" t="s">
         <v>54</v>
       </c>
@@ -3094,7 +3094,7 @@
       <c r="L72" s="76"/>
     </row>
     <row r="73" spans="1:12" s="27" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="134" t="s">
+      <c r="A73" s="170" t="s">
         <v>56</v>
       </c>
       <c r="B73" s="31" t="s">
@@ -3118,7 +3118,7 @@
       <c r="L73" s="76"/>
     </row>
     <row r="74" spans="1:12" s="27" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A74" s="135"/>
+      <c r="A74" s="171"/>
       <c r="B74" s="31" t="s">
         <v>54</v>
       </c>
@@ -3136,7 +3136,7 @@
       <c r="L74" s="76"/>
     </row>
     <row r="75" spans="1:12" s="27" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A75" s="135"/>
+      <c r="A75" s="171"/>
       <c r="B75" s="32" t="s">
         <v>60</v>
       </c>
@@ -3158,7 +3158,7 @@
       <c r="L75" s="76"/>
     </row>
     <row r="76" spans="1:12" s="25" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A76" s="136"/>
+      <c r="A76" s="172"/>
       <c r="B76" s="33" t="s">
         <v>54</v>
       </c>
@@ -3185,6 +3185,13 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A45:A56"/>
+    <mergeCell ref="G45:K45"/>
+    <mergeCell ref="A73:A76"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="A69:A72"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="G3:K5"/>
     <mergeCell ref="A7:F7"/>
@@ -3200,13 +3207,6 @@
     <mergeCell ref="A23:A44"/>
     <mergeCell ref="H23:J24"/>
     <mergeCell ref="I39:J39"/>
-    <mergeCell ref="A45:A56"/>
-    <mergeCell ref="G45:K45"/>
-    <mergeCell ref="A73:A76"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="A69:A72"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showErrorMessage="1" sqref="H46:H68 H71:J72 I55:J68"/>

</xml_diff>